<commit_message>
Mention RTC72421A as replacement
</commit_message>
<xml_diff>
--- a/docs/rejuvenator-bom.xlsx
+++ b/docs/rejuvenator-bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="186">
   <si>
     <t>Qty</t>
   </si>
@@ -166,6 +166,9 @@
     <t>OKI 6242B</t>
   </si>
   <si>
+    <t>Replacement: RTC72421A (do not populate Y1, C21, C24)</t>
+  </si>
+  <si>
     <t>DIP-18</t>
   </si>
   <si>
@@ -260,6 +263,9 @@
   </si>
   <si>
     <t>22pF</t>
+  </si>
+  <si>
+    <t>Skip if RTC72421A is used</t>
   </si>
   <si>
     <t>594-A220J15C0GH5TAA</t>
@@ -1281,11 +1287,14 @@
       <c r="B16" t="s">
         <v>49</v>
       </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1293,19 +1302,19 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1313,19 +1322,19 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1333,16 +1342,16 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1350,21 +1359,21 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
         <v>15</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1378,21 +1387,21 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1406,16 +1415,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1423,16 +1432,16 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D25" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1440,16 +1449,19 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="C26" t="s">
+        <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1457,16 +1469,16 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1474,13 +1486,13 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1488,21 +1500,24 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>91</v>
+      </c>
+      <c r="C29" t="s">
+        <v>83</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1516,16 +1531,16 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D31" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1533,16 +1548,16 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1550,16 +1565,16 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D33" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1567,16 +1582,16 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D34" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1584,16 +1599,16 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D35" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1601,16 +1616,16 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D36" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1618,16 +1633,16 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D37" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1635,21 +1650,21 @@
         <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D38" t="s">
         <v>19</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1663,21 +1678,24 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>119</v>
+        <v>121</v>
+      </c>
+      <c r="C40" t="s">
+        <v>83</v>
       </c>
       <c r="D40" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1691,13 +1709,13 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1705,10 +1723,10 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>21</v>
@@ -1719,13 +1737,13 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1733,13 +1751,13 @@
         <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1747,13 +1765,13 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1761,10 +1779,10 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>34</v>
@@ -1775,13 +1793,13 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1789,10 +1807,10 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>38</v>
@@ -1800,7 +1818,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1814,16 +1832,16 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C51" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1831,16 +1849,16 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C52" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1848,16 +1866,16 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C53" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1865,13 +1883,13 @@
         <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C54" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1879,13 +1897,13 @@
         <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C55" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1893,10 +1911,10 @@
         <v>6</v>
       </c>
       <c r="B56" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C56" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1904,13 +1922,13 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C57" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -1918,13 +1936,13 @@
         <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -1932,13 +1950,13 @@
         <v>4</v>
       </c>
       <c r="B59" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -1946,16 +1964,16 @@
         <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C60" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -1963,15 +1981,15 @@
         <v>2</v>
       </c>
       <c r="B61" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -1985,10 +2003,10 @@
         <v>1</v>
       </c>
       <c r="B63" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -1996,15 +2014,15 @@
         <v>3</v>
       </c>
       <c r="B64" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C64" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="60" customHeight="1">
       <c r="A66" s="5" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix remark on wrong component
</commit_message>
<xml_diff>
--- a/docs/rejuvenator-bom.xlsx
+++ b/docs/rejuvenator-bom.xlsx
@@ -590,7 +590,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Version: 0.2 (2023-06-02)
+      <t xml:space="preserve">Version: 0.3 (2023-06-02)
 </t>
     </r>
     <r>
@@ -1488,6 +1488,9 @@
       <c r="B28" t="s">
         <v>89</v>
       </c>
+      <c r="C28" t="s">
+        <v>83</v>
+      </c>
       <c r="D28" t="s">
         <v>75</v>
       </c>
@@ -1501,9 +1504,6 @@
       </c>
       <c r="B29" t="s">
         <v>91</v>
-      </c>
-      <c r="C29" t="s">
-        <v>83</v>
       </c>
       <c r="D29" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
Remarks about Agnus and Denise
</commit_message>
<xml_diff>
--- a/docs/rejuvenator-bom.xlsx
+++ b/docs/rejuvenator-bom.xlsx
@@ -148,7 +148,7 @@
     <t>Denise 8362</t>
   </si>
   <si>
-    <t>from your A1000, or 8373</t>
+    <t>from your A1000, or 8373 for ECS</t>
   </si>
   <si>
     <t>U25</t>
@@ -590,7 +590,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Version: 0.4 (2024-02-27)
+      <t xml:space="preserve">Version: 0.5 (2024-04-16)
 </t>
     </r>
     <r>

</xml_diff>